<commit_message>
adicionado tratamento de erros
</commit_message>
<xml_diff>
--- a/planilha/contatos.xlsx
+++ b/planilha/contatos.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Diogo</t>
   </si>
   <si>
-    <t xml:space="preserve">Flávio</t>
+    <t xml:space="preserve">Marciana</t>
   </si>
 </sst>
 </file>
@@ -146,10 +146,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
   </cols>
@@ -167,7 +167,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>5532999999999</v>
+        <v>5532988141424</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -175,7 +175,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5532999999999</v>
+        <v>5532988141424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>